<commit_message>
got coordinates for all of them!!!!!!!!!!!!!!!!!
</commit_message>
<xml_diff>
--- a/Surveys/2022/03_28_2022_Tracer_Survey.xlsx
+++ b/Surveys/2022/03_28_2022_Tracer_Survey.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\huck4481\Documents\GitHub\RFID_tracers\surveys\2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A57CAB3F-EEA6-4685-BFBF-E72D1C4FC606}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85D3289B-44C5-4703-BB85-B7F539FFF477}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{917B6B2B-C151-4D8F-993C-94E73463CAEA}"/>
+    <workbookView xWindow="-25320" yWindow="195" windowWidth="25440" windowHeight="15390" xr2:uid="{917B6B2B-C151-4D8F-993C-94E73463CAEA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -374,7 +374,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -398,10 +401,7 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -728,8 +728,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{436521EC-E644-46DF-BE23-F00DCF407353}">
   <dimension ref="A1:O110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A86" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="U102" sqref="U102"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -751,10 +751,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31"/>
+      <c r="B1" s="32"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
@@ -790,28 +790,28 @@
       <c r="A7" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="32" t="s">
+      <c r="B7" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="32"/>
-      <c r="D7" s="32"/>
-      <c r="E7" s="26" t="s">
+      <c r="C7" s="33"/>
+      <c r="D7" s="33"/>
+      <c r="E7" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="F7" s="26"/>
-      <c r="G7" s="26" t="s">
+      <c r="F7" s="35"/>
+      <c r="G7" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="H7" s="26"/>
-      <c r="I7" s="26"/>
-      <c r="J7" s="26"/>
-      <c r="K7" s="26"/>
-      <c r="L7" s="26" t="s">
+      <c r="H7" s="35"/>
+      <c r="I7" s="35"/>
+      <c r="J7" s="35"/>
+      <c r="K7" s="35"/>
+      <c r="L7" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="M7" s="26"/>
-      <c r="N7" s="26"/>
-      <c r="O7" s="26"/>
+      <c r="M7" s="35"/>
+      <c r="N7" s="35"/>
+      <c r="O7" s="35"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
@@ -1311,16 +1311,16 @@
       <c r="O26" s="25"/>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A27" s="34">
+      <c r="A27" s="26">
         <v>1050</v>
       </c>
-      <c r="B27" s="34" t="s">
-        <v>4</v>
-      </c>
-      <c r="C27" s="34" t="s">
-        <v>4</v>
-      </c>
-      <c r="D27" s="34" t="s">
+      <c r="B27" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="C27" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="D27" s="26" t="s">
         <v>4</v>
       </c>
       <c r="E27" s="19"/>
@@ -1336,16 +1336,16 @@
       <c r="O27" s="25"/>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A28" s="34">
+      <c r="A28" s="26">
         <v>1026</v>
       </c>
-      <c r="B28" s="34" t="s">
-        <v>4</v>
-      </c>
-      <c r="C28" s="34" t="s">
-        <v>4</v>
-      </c>
-      <c r="D28" s="34" t="s">
+      <c r="B28" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="C28" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="D28" s="26" t="s">
         <v>4</v>
       </c>
       <c r="E28" s="19"/>
@@ -1361,16 +1361,16 @@
       <c r="O28" s="25"/>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A29" s="34">
+      <c r="A29" s="26">
         <v>1055</v>
       </c>
-      <c r="B29" s="34">
+      <c r="B29" s="26">
         <v>108</v>
       </c>
-      <c r="C29" s="34">
+      <c r="C29" s="26">
         <v>165</v>
       </c>
-      <c r="D29" s="34">
+      <c r="D29" s="26">
         <v>184</v>
       </c>
       <c r="E29" s="19"/>
@@ -1386,16 +1386,16 @@
       <c r="O29" s="25"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A30" s="34">
+      <c r="A30" s="26">
         <v>1037</v>
       </c>
-      <c r="B30" s="34" t="s">
-        <v>4</v>
-      </c>
-      <c r="C30" s="34" t="s">
-        <v>4</v>
-      </c>
-      <c r="D30" s="34" t="s">
+      <c r="B30" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="C30" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="D30" s="26" t="s">
         <v>4</v>
       </c>
       <c r="E30" s="19"/>
@@ -1414,28 +1414,28 @@
       <c r="A32" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="B32" s="33" t="s">
+      <c r="B32" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="C32" s="33"/>
-      <c r="D32" s="33"/>
-      <c r="E32" s="26" t="s">
+      <c r="C32" s="34"/>
+      <c r="D32" s="34"/>
+      <c r="E32" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="F32" s="26"/>
-      <c r="G32" s="26" t="s">
+      <c r="F32" s="35"/>
+      <c r="G32" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="H32" s="26"/>
-      <c r="I32" s="26"/>
-      <c r="J32" s="26"/>
-      <c r="K32" s="26"/>
-      <c r="L32" s="26" t="s">
+      <c r="H32" s="35"/>
+      <c r="I32" s="35"/>
+      <c r="J32" s="35"/>
+      <c r="K32" s="35"/>
+      <c r="L32" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="M32" s="26"/>
-      <c r="N32" s="26"/>
-      <c r="O32" s="26"/>
+      <c r="M32" s="35"/>
+      <c r="N32" s="35"/>
+      <c r="O32" s="35"/>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
@@ -1785,16 +1785,16 @@
       <c r="O45" s="25"/>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A46" s="34">
+      <c r="A46" s="26">
         <v>1017</v>
       </c>
-      <c r="B46" s="34">
+      <c r="B46" s="26">
         <v>138</v>
       </c>
-      <c r="C46" s="34">
+      <c r="C46" s="26">
         <v>124</v>
       </c>
-      <c r="D46" s="34">
+      <c r="D46" s="26">
         <v>106</v>
       </c>
       <c r="E46" s="19"/>
@@ -1810,16 +1810,16 @@
       <c r="O46" s="25"/>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A47" s="34">
+      <c r="A47" s="26">
         <v>1036</v>
       </c>
-      <c r="B47" s="34">
+      <c r="B47" s="26">
         <v>134</v>
       </c>
-      <c r="C47" s="34">
+      <c r="C47" s="26">
         <v>129</v>
       </c>
-      <c r="D47" s="34">
+      <c r="D47" s="26">
         <v>101</v>
       </c>
       <c r="E47" s="19"/>
@@ -1835,16 +1835,16 @@
       <c r="O47" s="25"/>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A48" s="34">
+      <c r="A48" s="26">
         <v>1044</v>
       </c>
-      <c r="B48" s="34">
+      <c r="B48" s="26">
         <v>119</v>
       </c>
-      <c r="C48" s="34">
+      <c r="C48" s="26">
         <v>130</v>
       </c>
-      <c r="D48" s="34">
+      <c r="D48" s="26">
         <v>106</v>
       </c>
       <c r="E48" s="19"/>
@@ -1860,16 +1860,16 @@
       <c r="O48" s="25"/>
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A49" s="34">
+      <c r="A49" s="26">
         <v>1065</v>
       </c>
-      <c r="B49" s="34">
+      <c r="B49" s="26">
         <v>139</v>
       </c>
-      <c r="C49" s="34">
+      <c r="C49" s="26">
         <v>137</v>
       </c>
-      <c r="D49" s="34">
+      <c r="D49" s="26">
         <v>92</v>
       </c>
       <c r="E49" s="19"/>
@@ -1888,28 +1888,28 @@
       <c r="A51" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="B51" s="27" t="s">
+      <c r="B51" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="C51" s="27"/>
-      <c r="D51" s="28"/>
-      <c r="E51" s="26" t="s">
+      <c r="C51" s="28"/>
+      <c r="D51" s="29"/>
+      <c r="E51" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="F51" s="26"/>
-      <c r="G51" s="26" t="s">
+      <c r="F51" s="35"/>
+      <c r="G51" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="H51" s="26"/>
-      <c r="I51" s="26"/>
-      <c r="J51" s="26"/>
-      <c r="K51" s="26"/>
-      <c r="L51" s="26" t="s">
+      <c r="H51" s="35"/>
+      <c r="I51" s="35"/>
+      <c r="J51" s="35"/>
+      <c r="K51" s="35"/>
+      <c r="L51" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="M51" s="26"/>
-      <c r="N51" s="26"/>
-      <c r="O51" s="26"/>
+      <c r="M51" s="35"/>
+      <c r="N51" s="35"/>
+      <c r="O51" s="35"/>
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A52" s="6" t="s">
@@ -2334,16 +2334,16 @@
       <c r="O67" s="25"/>
     </row>
     <row r="68" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A68" s="34">
+      <c r="A68" s="26">
         <v>1006</v>
       </c>
-      <c r="B68" s="34" t="s">
-        <v>4</v>
-      </c>
-      <c r="C68" s="34" t="s">
-        <v>4</v>
-      </c>
-      <c r="D68" s="35" t="s">
+      <c r="B68" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="C68" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="D68" s="27" t="s">
         <v>4</v>
       </c>
       <c r="E68" s="19"/>
@@ -2359,16 +2359,16 @@
       <c r="O68" s="25"/>
     </row>
     <row r="69" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A69" s="34">
+      <c r="A69" s="26">
         <v>1011</v>
       </c>
-      <c r="B69" s="34" t="s">
-        <v>4</v>
-      </c>
-      <c r="C69" s="34" t="s">
-        <v>4</v>
-      </c>
-      <c r="D69" s="35" t="s">
+      <c r="B69" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="C69" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="D69" s="27" t="s">
         <v>4</v>
       </c>
       <c r="E69" s="19"/>
@@ -2384,16 +2384,16 @@
       <c r="O69" s="25"/>
     </row>
     <row r="70" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A70" s="34">
+      <c r="A70" s="26">
         <v>1048</v>
       </c>
-      <c r="B70" s="34">
+      <c r="B70" s="26">
         <v>81</v>
       </c>
-      <c r="C70" s="34">
+      <c r="C70" s="26">
         <v>138</v>
       </c>
-      <c r="D70" s="35">
+      <c r="D70" s="27">
         <v>325</v>
       </c>
       <c r="E70" s="19"/>
@@ -2409,16 +2409,16 @@
       <c r="O70" s="25"/>
     </row>
     <row r="71" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A71" s="34">
+      <c r="A71" s="26">
         <v>1062</v>
       </c>
-      <c r="B71" s="34">
+      <c r="B71" s="26">
         <v>168</v>
       </c>
-      <c r="C71" s="34">
+      <c r="C71" s="26">
         <v>34</v>
       </c>
-      <c r="D71" s="35">
+      <c r="D71" s="27">
         <v>281</v>
       </c>
       <c r="E71" s="19"/>
@@ -2437,28 +2437,28 @@
       <c r="A73" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="B73" s="29" t="s">
+      <c r="B73" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="C73" s="29"/>
-      <c r="D73" s="29"/>
-      <c r="E73" s="26" t="s">
+      <c r="C73" s="30"/>
+      <c r="D73" s="30"/>
+      <c r="E73" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="F73" s="26"/>
-      <c r="G73" s="26" t="s">
+      <c r="F73" s="35"/>
+      <c r="G73" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="H73" s="26"/>
-      <c r="I73" s="26"/>
-      <c r="J73" s="26"/>
-      <c r="K73" s="26"/>
-      <c r="L73" s="26" t="s">
+      <c r="H73" s="35"/>
+      <c r="I73" s="35"/>
+      <c r="J73" s="35"/>
+      <c r="K73" s="35"/>
+      <c r="L73" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="M73" s="26"/>
-      <c r="N73" s="26"/>
-      <c r="O73" s="26"/>
+      <c r="M73" s="35"/>
+      <c r="N73" s="35"/>
+      <c r="O73" s="35"/>
     </row>
     <row r="74" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A74" s="6" t="s">
@@ -2833,16 +2833,16 @@
       <c r="O87" s="25"/>
     </row>
     <row r="88" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A88" s="34">
+      <c r="A88" s="26">
         <v>1039</v>
       </c>
-      <c r="B88" s="34" t="s">
-        <v>4</v>
-      </c>
-      <c r="C88" s="34" t="s">
-        <v>4</v>
-      </c>
-      <c r="D88" s="34" t="s">
+      <c r="B88" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="C88" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="D88" s="26" t="s">
         <v>4</v>
       </c>
       <c r="E88" s="19"/>
@@ -2858,16 +2858,16 @@
       <c r="O88" s="25"/>
     </row>
     <row r="89" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A89" s="34">
+      <c r="A89" s="26">
         <v>1005</v>
       </c>
-      <c r="B89" s="34" t="s">
-        <v>4</v>
-      </c>
-      <c r="C89" s="34" t="s">
-        <v>4</v>
-      </c>
-      <c r="D89" s="34" t="s">
+      <c r="B89" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="C89" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="D89" s="26" t="s">
         <v>4</v>
       </c>
       <c r="E89" s="19"/>
@@ -2883,16 +2883,16 @@
       <c r="O89" s="25"/>
     </row>
     <row r="90" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A90" s="34">
+      <c r="A90" s="26">
         <v>1031</v>
       </c>
-      <c r="B90" s="34" t="s">
-        <v>4</v>
-      </c>
-      <c r="C90" s="34" t="s">
-        <v>4</v>
-      </c>
-      <c r="D90" s="34" t="s">
+      <c r="B90" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="C90" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="D90" s="26" t="s">
         <v>4</v>
       </c>
       <c r="E90" s="19"/>
@@ -2908,16 +2908,16 @@
       <c r="O90" s="25"/>
     </row>
     <row r="91" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A91" s="34">
+      <c r="A91" s="26">
         <v>1010</v>
       </c>
-      <c r="B91" s="34" t="s">
-        <v>4</v>
-      </c>
-      <c r="C91" s="34" t="s">
-        <v>4</v>
-      </c>
-      <c r="D91" s="34" t="s">
+      <c r="B91" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="C91" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="D91" s="26" t="s">
         <v>4</v>
       </c>
       <c r="E91" s="19"/>
@@ -2936,28 +2936,28 @@
       <c r="A93" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="B93" s="30" t="s">
+      <c r="B93" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="C93" s="30"/>
-      <c r="D93" s="30"/>
-      <c r="E93" s="26" t="s">
+      <c r="C93" s="31"/>
+      <c r="D93" s="31"/>
+      <c r="E93" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="F93" s="26"/>
-      <c r="G93" s="26" t="s">
+      <c r="F93" s="35"/>
+      <c r="G93" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="H93" s="26"/>
-      <c r="I93" s="26"/>
-      <c r="J93" s="26"/>
-      <c r="K93" s="26"/>
-      <c r="L93" s="26" t="s">
+      <c r="H93" s="35"/>
+      <c r="I93" s="35"/>
+      <c r="J93" s="35"/>
+      <c r="K93" s="35"/>
+      <c r="L93" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="M93" s="26"/>
-      <c r="N93" s="26"/>
-      <c r="O93" s="26"/>
+      <c r="M93" s="35"/>
+      <c r="N93" s="35"/>
+      <c r="O93" s="35"/>
     </row>
     <row r="94" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A94" s="6" t="s">
@@ -3307,16 +3307,16 @@
       <c r="O106" s="25"/>
     </row>
     <row r="107" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A107" s="34">
+      <c r="A107" s="26">
         <v>1002</v>
       </c>
-      <c r="B107" s="34">
+      <c r="B107" s="26">
         <v>224</v>
       </c>
-      <c r="C107" s="34">
+      <c r="C107" s="26">
         <v>190</v>
       </c>
-      <c r="D107" s="34">
+      <c r="D107" s="26">
         <v>107</v>
       </c>
       <c r="E107" s="19"/>
@@ -3332,16 +3332,16 @@
       <c r="O107" s="25"/>
     </row>
     <row r="108" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A108" s="34">
+      <c r="A108" s="26">
         <v>1014</v>
       </c>
-      <c r="B108" s="34">
+      <c r="B108" s="26">
         <v>202</v>
       </c>
-      <c r="C108" s="34">
+      <c r="C108" s="26">
         <v>159</v>
       </c>
-      <c r="D108" s="34">
+      <c r="D108" s="26">
         <v>89</v>
       </c>
       <c r="E108" s="19"/>
@@ -3357,16 +3357,16 @@
       <c r="O108" s="25"/>
     </row>
     <row r="109" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A109" s="34">
+      <c r="A109" s="26">
         <v>1043</v>
       </c>
-      <c r="B109" s="34">
+      <c r="B109" s="26">
         <v>168</v>
       </c>
-      <c r="C109" s="34">
+      <c r="C109" s="26">
         <v>115</v>
       </c>
-      <c r="D109" s="34">
+      <c r="D109" s="26">
         <v>85</v>
       </c>
       <c r="E109" s="19"/>
@@ -3382,16 +3382,16 @@
       <c r="O109" s="25"/>
     </row>
     <row r="110" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A110" s="34">
+      <c r="A110" s="26">
         <v>1058</v>
       </c>
-      <c r="B110" s="34">
+      <c r="B110" s="26">
         <v>191</v>
       </c>
-      <c r="C110" s="34">
+      <c r="C110" s="26">
         <v>147</v>
       </c>
-      <c r="D110" s="34">
+      <c r="D110" s="26">
         <v>86</v>
       </c>
       <c r="E110" s="19"/>
@@ -3408,18 +3408,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="B51:D51"/>
-    <mergeCell ref="B73:D73"/>
-    <mergeCell ref="B93:D93"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="B32:D32"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="G7:K7"/>
-    <mergeCell ref="L7:O7"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="G32:K32"/>
-    <mergeCell ref="L32:O32"/>
     <mergeCell ref="E93:F93"/>
     <mergeCell ref="G93:K93"/>
     <mergeCell ref="L93:O93"/>
@@ -3429,6 +3417,18 @@
     <mergeCell ref="E73:F73"/>
     <mergeCell ref="G73:K73"/>
     <mergeCell ref="L73:O73"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="G7:K7"/>
+    <mergeCell ref="L7:O7"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="G32:K32"/>
+    <mergeCell ref="L32:O32"/>
+    <mergeCell ref="B51:D51"/>
+    <mergeCell ref="B73:D73"/>
+    <mergeCell ref="B93:D93"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B32:D32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>

</xml_diff>